<commit_message>
Pushes to update IG
</commit_message>
<xml_diff>
--- a/StructureDefinition-cbs-composition.xlsx
+++ b/StructureDefinition-cbs-composition.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$209</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$223</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7590" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8099" uniqueCount="450">
   <si>
     <t>Path</t>
   </si>
@@ -1349,6 +1349,16 @@
   </si>
   <si>
     <t>Composition.section.section.section</t>
+  </si>
+  <si>
+    <t>reporting</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://cbsig.chai.gatech.edu/StructureDefinition/cbs-person-reporting-to-cdc|http://cbsig.chai.gatech.edu/StructureDefinition/cbs-reporting-source-organization)
+</t>
   </si>
   <si>
     <t>epi</t>
@@ -1555,7 +1565,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN209"/>
+  <dimension ref="A1:AN223"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -22033,7 +22043,7 @@
         <v>41</v>
       </c>
       <c r="J179" t="s" s="2">
-        <v>325</v>
+        <v>443</v>
       </c>
       <c r="K179" t="s" s="2">
         <v>386</v>
@@ -22357,7 +22367,7 @@
         <v>329</v>
       </c>
       <c r="B182" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C182" t="s" s="2">
         <v>41</v>
@@ -22855,7 +22865,7 @@
         <v>41</v>
       </c>
       <c r="R186" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="S186" t="s" s="2">
         <v>41</v>
@@ -23963,7 +23973,7 @@
         <v>329</v>
       </c>
       <c r="B196" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C196" t="s" s="2">
         <v>41</v>
@@ -24461,7 +24471,7 @@
         <v>41</v>
       </c>
       <c r="R200" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="S200" t="s" s="2">
         <v>41</v>
@@ -25564,8 +25574,1614 @@
         <v>41</v>
       </c>
     </row>
+    <row r="210">
+      <c r="A210" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="B210" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="C210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D210" s="2"/>
+      <c r="E210" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F210" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G210" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="H210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J210" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="K210" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="L210" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="M210" s="2"/>
+      <c r="N210" s="2"/>
+      <c r="O210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P210" s="2"/>
+      <c r="Q210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE210" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="AF210" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG210" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI210" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AJ210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK210" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AL210" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AM210" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN210" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="211" hidden="true">
+      <c r="A211" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="B211" s="2"/>
+      <c r="C211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D211" s="2"/>
+      <c r="E211" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F211" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J211" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="K211" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="L211" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="M211" s="2"/>
+      <c r="N211" s="2"/>
+      <c r="O211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P211" s="2"/>
+      <c r="Q211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE211" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="AF211" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG211" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK211" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AL211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AM211" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN211" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="212" hidden="true">
+      <c r="A212" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="B212" s="2"/>
+      <c r="C212" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="D212" s="2"/>
+      <c r="E212" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F212" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J212" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="K212" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="L212" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="M212" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="N212" s="2"/>
+      <c r="O212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P212" s="2"/>
+      <c r="Q212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE212" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AF212" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG212" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI212" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK212" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AL212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AM212" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN212" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="213" hidden="true">
+      <c r="A213" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="B213" s="2"/>
+      <c r="C213" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="D213" s="2"/>
+      <c r="E213" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F213" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H213" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="I213" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J213" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="K213" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="L213" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="M213" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="N213" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="O213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P213" s="2"/>
+      <c r="Q213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE213" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AF213" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG213" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI213" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AJ213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK213" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AL213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AM213" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN213" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="214" hidden="true">
+      <c r="A214" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="B214" s="2"/>
+      <c r="C214" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="D214" s="2"/>
+      <c r="E214" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="F214" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J214" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="K214" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="L214" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="M214" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="N214" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="O214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P214" s="2"/>
+      <c r="Q214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R214" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="S214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE214" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="AF214" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG214" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI214" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK214" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="AL214" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="AM214" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN214" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="215" hidden="true">
+      <c r="A215" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="B215" s="2"/>
+      <c r="C215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D215" s="2"/>
+      <c r="E215" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F215" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J215" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="K215" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="L215" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="M215" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="N215" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="O215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P215" s="2"/>
+      <c r="Q215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W215" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="X215" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="Y215" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="Z215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE215" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AF215" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG215" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI215" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK215" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AL215" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="AM215" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN215" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="216" hidden="true">
+      <c r="A216" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="B216" s="2"/>
+      <c r="C216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D216" s="2"/>
+      <c r="E216" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F216" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J216" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="K216" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L216" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="M216" s="2"/>
+      <c r="N216" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="O216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P216" s="2"/>
+      <c r="Q216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE216" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="AF216" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG216" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI216" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK216" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL216" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="AM216" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN216" t="s" s="2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="217" hidden="true">
+      <c r="A217" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="B217" s="2"/>
+      <c r="C217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D217" s="2"/>
+      <c r="E217" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F217" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J217" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="K217" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="L217" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="M217" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="N217" s="2"/>
+      <c r="O217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P217" s="2"/>
+      <c r="Q217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE217" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AF217" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG217" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI217" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AL217" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="AM217" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN217" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="218" hidden="true">
+      <c r="A218" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="B218" s="2"/>
+      <c r="C218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D218" s="2"/>
+      <c r="E218" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F218" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J218" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="K218" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="L218" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="M218" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="N218" s="2"/>
+      <c r="O218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P218" s="2"/>
+      <c r="Q218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE218" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="AF218" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG218" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH218" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AI218" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK218" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AL218" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AM218" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN218" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="219" hidden="true">
+      <c r="A219" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="B219" s="2"/>
+      <c r="C219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D219" s="2"/>
+      <c r="E219" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F219" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J219" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="K219" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="L219" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="M219" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="N219" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="O219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P219" s="2"/>
+      <c r="Q219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W219" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="X219" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="Y219" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="Z219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE219" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="AF219" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG219" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI219" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK219" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="AL219" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AM219" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN219" t="s" s="2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="220" hidden="true">
+      <c r="A220" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="B220" s="2"/>
+      <c r="C220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D220" s="2"/>
+      <c r="E220" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F220" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J220" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="K220" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="L220" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="M220" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="N220" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="O220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P220" s="2"/>
+      <c r="Q220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W220" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X220" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="Y220" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="Z220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE220" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="AF220" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG220" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI220" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK220" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AL220" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AM220" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN220" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="221" hidden="true">
+      <c r="A221" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="B221" s="2"/>
+      <c r="C221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D221" s="2"/>
+      <c r="E221" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F221" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J221" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="K221" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="L221" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="M221" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="N221" s="2"/>
+      <c r="O221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P221" s="2"/>
+      <c r="Q221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE221" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="AF221" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG221" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH221" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AI221" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK221" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AL221" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="AM221" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN221" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="222" hidden="true">
+      <c r="A222" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="B222" s="2"/>
+      <c r="C222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D222" s="2"/>
+      <c r="E222" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F222" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J222" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="K222" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L222" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="M222" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="N222" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="O222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P222" s="2"/>
+      <c r="Q222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W222" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X222" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="Y222" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="Z222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE222" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="AF222" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG222" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AH222" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AI222" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK222" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="AL222" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AM222" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN222" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="223" hidden="true">
+      <c r="A223" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="B223" s="2"/>
+      <c r="C223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D223" s="2"/>
+      <c r="E223" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F223" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="K223" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="L223" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="M223" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="N223" s="2"/>
+      <c r="O223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P223" s="2"/>
+      <c r="Q223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE223" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="AF223" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG223" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH223" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AI223" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AJ223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK223" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AL223" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="AM223" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AN223" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AN209">
+  <autoFilter ref="A1:AN223">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -25575,7 +27191,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI208">
+  <conditionalFormatting sqref="A2:AI222">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>